<commit_message>
Routenberechnung auf OpenRouteService umgestellt, Transporthäufigkeit summiert, Google Maps-Links hinzugefügt
</commit_message>
<xml_diff>
--- a/Datenblatt Routenanalyse .xlsx
+++ b/Datenblatt Routenanalyse .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BEV_Routen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FD4933-ECE1-4D42-A5AB-293D66A082F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC61D48-276E-4C3C-BD3F-F37CB2555880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{83282695-DF03-4A63-966C-62B2AB7565CF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="160">
   <si>
     <t>Route</t>
   </si>
@@ -77,9 +77,6 @@
     <t>DE 38239</t>
   </si>
   <si>
-    <t>52.1500	; 10.3333</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/tgd6st99aTHangMj8</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>DE 96476</t>
   </si>
   <si>
-    <t>50.3500	; 10.8000</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/UbtkX2jtsV2x55259</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>PL 39-442</t>
   </si>
   <si>
-    <t>50.5667; 21.6667</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/rKU3M73xUuro4ypM8</t>
   </si>
   <si>
@@ -125,9 +116,6 @@
     <t>DE 88046</t>
   </si>
   <si>
-    <t>47.6500; 9.4833</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/bjHmGCvqRQDMDS7o9</t>
   </si>
   <si>
@@ -137,9 +125,6 @@
     <t>DE 76703</t>
   </si>
   <si>
-    <t>49.1333; 8.7000</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/eL5epCmj5h5EMBVs5</t>
   </si>
   <si>
@@ -149,9 +134,6 @@
     <t>HU 9155</t>
   </si>
   <si>
-    <t>47.8000; 17.4167</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/zMWtBJZh5eWc2B437</t>
   </si>
   <si>
@@ -161,9 +143,6 @@
     <t>DE 93333</t>
   </si>
   <si>
-    <t>48.8000; 11.7667</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/8qLMAiGhAFAHnAk8A</t>
   </si>
   <si>
@@ -173,9 +152,6 @@
     <t>CZ 322 00</t>
   </si>
   <si>
-    <t>49.7500; 13.3667</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/G4iz7VA8yHv6cTX67</t>
   </si>
   <si>
@@ -185,9 +161,6 @@
     <t>DE 96257</t>
   </si>
   <si>
-    <t>50.1667; 11.2167</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/9QZioDu6VRCsRuQv6</t>
   </si>
   <si>
@@ -197,9 +170,6 @@
     <t>AT 3193</t>
   </si>
   <si>
-    <t>47.8667; 15.4667</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/mHbn7GTKSLDwWyV36</t>
   </si>
   <si>
@@ -209,9 +179,6 @@
     <t>PL 27200</t>
   </si>
   <si>
-    <t>51.0667; 21.0667</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/TLAXPL52Qiv9kNhs5</t>
   </si>
   <si>
@@ -221,9 +188,6 @@
     <t>AT 4400</t>
   </si>
   <si>
-    <t>48.0500; 14.4167</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/i5BSybpb6NnTBCoJ9</t>
   </si>
   <si>
@@ -233,9 +197,6 @@
     <t>DE 94315</t>
   </si>
   <si>
-    <t>48.8833; 12.5667</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/9W6hCDaY59EHk8Po8</t>
   </si>
   <si>
@@ -245,9 +206,6 @@
     <t>PL 49-318</t>
   </si>
   <si>
-    <t>50.7500; 17.6500</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/16CXn3in8LgvoAyh6</t>
   </si>
   <si>
@@ -257,9 +215,6 @@
     <t>DE 90402</t>
   </si>
   <si>
-    <t>49.4500; 11.0833</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/C5St1xbuoYJ9y7ATA</t>
   </si>
   <si>
@@ -269,9 +224,6 @@
     <t>PL 62300</t>
   </si>
   <si>
-    <t>52.3167; 17.5667</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/YX24Ra3vJnhD3An78</t>
   </si>
   <si>
@@ -284,7 +236,7 @@
     <t>PL 32-005</t>
   </si>
   <si>
-    <t>47.8833; 11.9167</t>
+    <t>50.0333; 	20.2167</t>
   </si>
   <si>
     <t>https://maps.app.goo.gl/sbnkuQAZGMSHyMhx9</t>
@@ -296,9 +248,6 @@
     <t>DE 91465</t>
   </si>
   <si>
-    <t>49.5333; 10.3333</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/RpQQybmxkPBfcJem7</t>
   </si>
   <si>
@@ -308,9 +257,6 @@
     <t>DE 65462</t>
   </si>
   <si>
-    <t>49.9667; 8.3333</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/MqWGurWvdqWsVfsz6</t>
   </si>
   <si>
@@ -320,9 +266,6 @@
     <t>DE 30159</t>
   </si>
   <si>
-    <t>52.3667; 9.7333</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/2EbtSHeWyndnZXg6A</t>
   </si>
   <si>
@@ -350,9 +293,6 @@
     <t>DE 83022</t>
   </si>
   <si>
-    <t>47.8500; 12.1333</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/z1F9VxVYzN46AxBQ6</t>
   </si>
   <si>
@@ -368,9 +308,6 @@
     <t>IT 13048</t>
   </si>
   <si>
-    <t>45.3667; 8.1667</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/W3BPcDhqFnvKJP9f9</t>
   </si>
   <si>
@@ -380,9 +317,6 @@
     <t>DE 86529</t>
   </si>
   <si>
-    <t>48.5667; 11.2667</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/KZcgh56X7Yjk6LEM8</t>
   </si>
   <si>
@@ -398,9 +332,6 @@
     <t>DE 85254</t>
   </si>
   <si>
-    <t>48.2833; 11.2667</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/qzrXrf1VdX7veDA8A</t>
   </si>
   <si>
@@ -413,12 +344,6 @@
     <t>DE 90441</t>
   </si>
   <si>
-    <t>50.8333; 10.9500</t>
-  </si>
-  <si>
-    <t>49.4167; 11.0833</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/UjnPzQhkkgxhf2B6A</t>
   </si>
   <si>
@@ -434,10 +359,215 @@
     <t>https://maps.app.goo.gl/ZVHL4rgXBV6ZGfB3A</t>
   </si>
   <si>
-    <t>48.2167; 11.5667</t>
-  </si>
-  <si>
-    <t>50.0333; 20.2167</t>
+    <t>Anschrift Lieferant</t>
+  </si>
+  <si>
+    <t>Dachauer Straße 667
+80995 München
+Deutschland</t>
+  </si>
+  <si>
+    <t>11.477112, 48.218301</t>
+  </si>
+  <si>
+    <t>10.424654, 52.145802</t>
+  </si>
+  <si>
+    <t>Werner-von-Siemens-Straße 6
+96476 Bad Rodach
+Deutschland</t>
+  </si>
+  <si>
+    <t>10.787276, 50.336515</t>
+  </si>
+  <si>
+    <t>Strefowa 17
+39-442 Chmielow
+Polen</t>
+  </si>
+  <si>
+    <t>21.634461, 50.518416</t>
+  </si>
+  <si>
+    <t>Alfred Colsman Platz 1
+88046 Friedrichshafen
+Deutschland</t>
+  </si>
+  <si>
+    <t>9.473924338817598, 47.661521606318324</t>
+  </si>
+  <si>
+    <t>Alte Münzesheimerstr. 4
+76703 Kraichtal- Gochsheim
+Deutschland</t>
+  </si>
+  <si>
+    <t>8.742357194423677, 49.1091986739026</t>
+  </si>
+  <si>
+    <t>Göbeház park 8.
+9155 Lébény
+Ungarn</t>
+  </si>
+  <si>
+    <t>17.41315305233002, 47.747338823683016</t>
+  </si>
+  <si>
+    <t>Umbertshausener Weg 7 
+93333 Neustadt an der Donau 
+Deutschland</t>
+  </si>
+  <si>
+    <t>11.709476, 48.763547</t>
+  </si>
+  <si>
+    <t>Pod Kyjovem 18
+32200 Plzeň - Radčice 
+Tschechische Republik</t>
+  </si>
+  <si>
+    <t>13.318127989768984, 49.766006885387156</t>
+  </si>
+  <si>
+    <t>Dorfstraße 74
+96257 Redwitz / Unterlangenstadt
+Deutschland</t>
+  </si>
+  <si>
+    <t>11.233853101730347, 50.1784200142913</t>
+  </si>
+  <si>
+    <t>Eisenwerk 14
+3193 St. Aegyd A.N.
+Österreich</t>
+  </si>
+  <si>
+    <t>15.58067321777344, 47.85994221398225</t>
+  </si>
+  <si>
+    <t>ul. Skladowa 33  
+27-200 Starachowice
+Polen</t>
+  </si>
+  <si>
+    <t>21.07138305902481, 51.07032287012852</t>
+  </si>
+  <si>
+    <t>Schönauerstraße 5
+4400 Steyr
+Österreich</t>
+  </si>
+  <si>
+    <t>14.427454, 48.039185</t>
+  </si>
+  <si>
+    <t>Stettiner Str. 7
+94315 Straubing
+Deutschland</t>
+  </si>
+  <si>
+    <t>12.614424, 48.88921</t>
+  </si>
+  <si>
+    <t>ul. Motorzycacyjna 1 
+49-318 SKARBIMIERZ
+Polen</t>
+  </si>
+  <si>
+    <t>17.424667775630954, 50.83476996821046</t>
+  </si>
+  <si>
+    <t>Vogelweiherstraße 33 
+90441 Nürnberg
+Deutschland</t>
+  </si>
+  <si>
+    <t>11.072628, 49.425104</t>
+  </si>
+  <si>
+    <t>ul. Działkowców 12
+62-300 Września
+Polen</t>
+  </si>
+  <si>
+    <t>17.54873335361481, 52.32382570067544</t>
+  </si>
+  <si>
+    <t>Heimatweg 84
+83052 Bruckmühl
+Deutschland</t>
+  </si>
+  <si>
+    <t>11.953715085983278, 47.87133432631062</t>
+  </si>
+  <si>
+    <t>Buchheimer Str. 4
+91465 Ergersheim
+Deutschland</t>
+  </si>
+  <si>
+    <t>10.325303077697756, 49.50718507184477</t>
+  </si>
+  <si>
+    <t>Ginsheimer Straße 2  
+65462 Ginsheim-Gustavsburg  
+Deutschland</t>
+  </si>
+  <si>
+    <t>8.325206637382509, 49.99184627801866</t>
+  </si>
+  <si>
+    <t>Am Leineufer 51
+30419 Hannover
+Deutschland</t>
+  </si>
+  <si>
+    <t>9.633076, 52.416928</t>
+  </si>
+  <si>
+    <t>Simsseestraße 15 
+83022 Rosenheim
+Deutschland</t>
+  </si>
+  <si>
+    <t>12.142148, 47.852512</t>
+  </si>
+  <si>
+    <t>Heinrich-Büssing-Straße 1
+38239 Salzgitter
+Deutschland</t>
+  </si>
+  <si>
+    <t>Via Guido Rossa 1
+13048 Santhià VC 
+Italien</t>
+  </si>
+  <si>
+    <t>8.182408, 45.368216</t>
+  </si>
+  <si>
+    <t>Lauterbacher Weg 2a 
+86529 Schrobenhausen
+Deutschland</t>
+  </si>
+  <si>
+    <t>11.290182, 48.563283</t>
+  </si>
+  <si>
+    <t>Maffeistraße 8
+85254 Sulzemoos
+Deutschland</t>
+  </si>
+  <si>
+    <t>11.259164, 48.281499</t>
+  </si>
+  <si>
+    <t>Robert-Bosch-Straße 1
+99310 Arnstadt
+Deutschland</t>
+  </si>
+  <si>
+    <t>10.948379, 50.86158</t>
   </si>
 </sst>
 </file>
@@ -564,7 +694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -587,8 +717,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -925,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46FEC3A-5B58-4AC6-B631-3EB971BEE35A}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -939,1132 +1072,1234 @@
     <col min="7" max="7" width="48.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="51" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1</v>
+      <c r="E2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="G2" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H2" s="5">
         <v>5</v>
       </c>
       <c r="I2" s="5">
+        <v>5</v>
+      </c>
+      <c r="J2" s="5">
         <v>10</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="5">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>33</v>
+      </c>
+      <c r="I3" s="5">
+        <v>5</v>
+      </c>
+      <c r="J3" s="5">
+        <v>38</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="5">
-        <v>2</v>
-      </c>
-      <c r="G3" s="5">
-        <v>33</v>
-      </c>
-      <c r="H3" s="5">
-        <v>5</v>
-      </c>
-      <c r="I3" s="5">
-        <v>38</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F4" s="5">
-        <v>1</v>
+      <c r="E4" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G4" s="5">
-        <v>10.5</v>
+        <v>1</v>
       </c>
       <c r="H4" s="5">
         <v>10.5</v>
       </c>
       <c r="I4" s="5">
+        <v>10.5</v>
+      </c>
+      <c r="J4" s="5">
         <v>21</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
+      <c r="E5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G5" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="5">
         <v>2</v>
       </c>
       <c r="I5" s="5">
+        <v>2</v>
+      </c>
+      <c r="J5" s="5">
         <v>4</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" s="5">
-        <v>1</v>
+      <c r="E6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G6" s="5">
-        <v>17.5</v>
+        <v>1</v>
       </c>
       <c r="H6" s="5">
         <v>17.5</v>
       </c>
       <c r="I6" s="5">
+        <v>17.5</v>
+      </c>
+      <c r="J6" s="5">
         <v>35</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1</v>
+      <c r="E7" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G7" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5">
         <v>4</v>
       </c>
       <c r="I7" s="5">
+        <v>4</v>
+      </c>
+      <c r="J7" s="5">
         <v>8</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>119</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
+      <c r="E8" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G8" s="5">
-        <v>8.5</v>
+        <v>1</v>
       </c>
       <c r="H8" s="5">
         <v>8.5</v>
       </c>
       <c r="I8" s="5">
+        <v>8.5</v>
+      </c>
+      <c r="J8" s="5">
         <v>17</v>
       </c>
-      <c r="J8" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>121</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1</v>
+      <c r="E9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G9" s="5">
-        <v>10.5</v>
+        <v>1</v>
       </c>
       <c r="H9" s="5">
         <v>10.5</v>
       </c>
       <c r="I9" s="5">
+        <v>10.5</v>
+      </c>
+      <c r="J9" s="5">
         <v>21</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>123</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="E10" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="5">
         <v>2</v>
-      </c>
-      <c r="G10" s="5">
-        <v>6</v>
       </c>
       <c r="H10" s="5">
         <v>6</v>
       </c>
       <c r="I10" s="5">
+        <v>6</v>
+      </c>
+      <c r="J10" s="5">
         <v>12</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
+      <c r="E11" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G11" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="5">
         <v>2</v>
       </c>
       <c r="I11" s="5">
+        <v>2</v>
+      </c>
+      <c r="J11" s="5">
         <v>4</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>52</v>
+        <v>42</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>127</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1</v>
+      <c r="E12" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G12" s="5">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="H12" s="5">
         <v>5.5</v>
       </c>
       <c r="I12" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="J12" s="5">
         <v>11</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>129</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F13" s="5">
-        <v>1</v>
+      <c r="E13" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G13" s="5">
-        <v>10.5</v>
+        <v>1</v>
       </c>
       <c r="H13" s="5">
         <v>10.5</v>
       </c>
       <c r="I13" s="5">
+        <v>10.5</v>
+      </c>
+      <c r="J13" s="5">
         <v>21</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>60</v>
+        <v>48</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="5">
         <v>2</v>
-      </c>
-      <c r="G14" s="5">
-        <v>35</v>
       </c>
       <c r="H14" s="5">
         <v>35</v>
       </c>
       <c r="I14" s="5">
+        <v>35</v>
+      </c>
+      <c r="J14" s="5">
         <v>70</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>64</v>
+        <v>51</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>133</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F15" s="5">
-        <v>1</v>
+      <c r="E15" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G15" s="5">
-        <v>10.5</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>10.5</v>
       </c>
       <c r="I15" s="5">
+        <v>10.5</v>
+      </c>
+      <c r="J15" s="5">
         <v>21</v>
       </c>
-      <c r="J15" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F16" s="5">
-        <v>1</v>
+      <c r="E16" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G16" s="5">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
         <v>21</v>
       </c>
       <c r="I16" s="5">
+        <v>21</v>
+      </c>
+      <c r="J16" s="5">
         <v>42</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>72</v>
+        <v>57</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>137</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F17" s="5">
-        <v>1</v>
+      <c r="E17" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G17" s="5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
         <v>1.5</v>
       </c>
       <c r="I17" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="J17" s="5">
         <v>3</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>76</v>
+        <v>60</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>139</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F18" s="5">
-        <v>1</v>
+      <c r="E18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="G18" s="5">
-        <v>73.5</v>
+        <v>1</v>
       </c>
       <c r="H18" s="5">
         <v>73.5</v>
       </c>
       <c r="I18" s="5">
+        <v>73.5</v>
+      </c>
+      <c r="J18" s="5">
         <v>147</v>
       </c>
-      <c r="J18" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>80</v>
+        <v>63</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F19" s="5">
+        <v>64</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="5">
         <v>2</v>
-      </c>
-      <c r="G19" s="5">
-        <v>87.5</v>
       </c>
       <c r="H19" s="5">
         <v>87.5</v>
       </c>
       <c r="I19" s="5">
+        <v>87.5</v>
+      </c>
+      <c r="J19" s="5">
         <v>175</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>85</v>
+        <v>68</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>143</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F20" s="5">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="G20" s="5">
-        <v>10.5</v>
+        <v>1</v>
       </c>
       <c r="H20" s="5">
         <v>10.5</v>
       </c>
       <c r="I20" s="5">
+        <v>10.5</v>
+      </c>
+      <c r="J20" s="5">
         <v>21</v>
       </c>
-      <c r="J20" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>89</v>
+        <v>71</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>145</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" s="5">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="G21" s="5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H21" s="5">
         <v>8</v>
       </c>
       <c r="I21" s="5">
+        <v>8</v>
+      </c>
+      <c r="J21" s="5">
         <v>16</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>147</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F22" s="5">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
         <v>10.5</v>
       </c>
-      <c r="H22" s="5">
+      <c r="I22" s="5">
         <v>7</v>
       </c>
-      <c r="I22" s="5">
+      <c r="J22" s="5">
         <v>17.5</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>32</v>
+        <v>77</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="G23" s="5">
-        <v>10.5</v>
+        <v>1</v>
       </c>
       <c r="H23" s="5">
         <v>10.5</v>
       </c>
       <c r="I23" s="5">
+        <v>10.5</v>
+      </c>
+      <c r="J23" s="5">
         <v>21</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="D24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="5">
+        <v>2</v>
+      </c>
+      <c r="H24" s="5">
+        <v>192.5</v>
+      </c>
+      <c r="I24" s="5">
+        <v>52.5</v>
+      </c>
+      <c r="J24" s="5">
+        <v>245</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F24" s="5">
-        <v>2</v>
-      </c>
-      <c r="G24" s="5">
-        <v>192.5</v>
-      </c>
-      <c r="H24" s="5">
-        <v>52.5</v>
-      </c>
-      <c r="I24" s="5">
-        <v>245</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>40</v>
+      <c r="B25" s="10" t="s">
+        <v>121</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F25" s="5">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="G25" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H25" s="5">
         <v>10</v>
       </c>
       <c r="I25" s="5">
+        <v>10</v>
+      </c>
+      <c r="J25" s="5">
         <v>20</v>
       </c>
-      <c r="J25" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>103</v>
+        <v>83</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>149</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F26" s="5">
+        <v>84</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="5">
         <v>2</v>
-      </c>
-      <c r="G26" s="5">
-        <v>66.5</v>
       </c>
       <c r="H26" s="5">
         <v>66.5</v>
       </c>
       <c r="I26" s="5">
+        <v>66.5</v>
+      </c>
+      <c r="J26" s="5">
         <v>133</v>
       </c>
-      <c r="J26" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B27" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F27" s="5">
-        <v>1</v>
+      <c r="D27" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="G27" s="5">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="H27" s="5">
         <v>35</v>
       </c>
       <c r="I27" s="5">
+        <v>35</v>
+      </c>
+      <c r="J27" s="5">
         <v>70</v>
       </c>
-      <c r="J27" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>109</v>
+        <v>88</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F28" s="5">
+        <v>89</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="5">
         <v>2</v>
-      </c>
-      <c r="G28" s="5">
-        <v>19.5</v>
       </c>
       <c r="H28" s="5">
         <v>19.5</v>
       </c>
       <c r="I28" s="5">
+        <v>19.5</v>
+      </c>
+      <c r="J28" s="5">
         <v>39</v>
       </c>
-      <c r="J28" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>113</v>
+        <v>91</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>154</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F29" s="5">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="G29" s="5">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5">
         <v>8.5</v>
       </c>
-      <c r="H29" s="5">
+      <c r="I29" s="5">
         <v>2.5</v>
       </c>
-      <c r="I29" s="5">
+      <c r="J29" s="5">
         <v>11</v>
       </c>
-      <c r="J29" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>60</v>
+        <v>94</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F30" s="5">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="G30" s="5">
-        <v>73.5</v>
+        <v>1</v>
       </c>
       <c r="H30" s="5">
         <v>73.5</v>
       </c>
       <c r="I30" s="5">
+        <v>73.5</v>
+      </c>
+      <c r="J30" s="5">
         <v>147</v>
       </c>
-      <c r="J30" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>119</v>
+        <v>96</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>156</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F31" s="5">
+        <v>97</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" s="5">
         <v>3</v>
-      </c>
-      <c r="G31" s="5">
-        <v>63</v>
       </c>
       <c r="H31" s="5">
         <v>63</v>
       </c>
       <c r="I31" s="5">
+        <v>63</v>
+      </c>
+      <c r="J31" s="5">
         <v>126</v>
       </c>
-      <c r="J31" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>123</v>
+        <v>99</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="F32" s="5">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="G32" s="5">
+        <v>1</v>
+      </c>
+      <c r="H32" s="5">
         <v>35</v>
       </c>
-      <c r="H32" s="5">
+      <c r="I32" s="5">
         <v>10.5</v>
       </c>
-      <c r="I32" s="5">
+      <c r="J32" s="5">
         <v>45.5</v>
       </c>
-      <c r="J32" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B33" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="5">
-        <v>1</v>
+      <c r="E33" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="G33" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H33" s="5">
         <v>5</v>
       </c>
       <c r="I33" s="5">
+        <v>5</v>
+      </c>
+      <c r="J33" s="5">
         <v>10</v>
       </c>
-      <c r="J33" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>60</v>
+        <v>105</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="8">
-        <v>1</v>
+      <c r="E34" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="G34" s="8">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="H34" s="8">
         <v>14</v>
       </c>
       <c r="I34" s="8">
+        <v>14</v>
+      </c>
+      <c r="J34" s="8">
         <v>28</v>
       </c>
-      <c r="J34" s="9" t="s">
-        <v>131</v>
+      <c r="K34" s="9" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{C58A20DA-B273-448D-BC95-979A40E9B571}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{DEC8F90F-0B44-45F4-A6DC-B683EE12D870}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{9F2D1D6E-5304-4E55-99D9-FF61FE89C727}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{B29EC484-2D7B-43AB-9377-E99C8E5ED81E}"/>
-    <hyperlink ref="J6" r:id="rId5" xr:uid="{0AB116EB-8B75-4CAF-8C0A-196E2288D377}"/>
-    <hyperlink ref="J7" r:id="rId6" xr:uid="{693B7AC2-5DD1-4E04-B8C9-9B1995410F31}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{BC115385-F150-439B-B52C-B49FB63F3125}"/>
-    <hyperlink ref="J9" r:id="rId8" xr:uid="{78B69A5A-8696-4C99-9BA9-542E11838C3C}"/>
-    <hyperlink ref="J10" r:id="rId9" xr:uid="{9B61FD39-2362-4E1A-9E4F-782588E2FE08}"/>
-    <hyperlink ref="J11" r:id="rId10" xr:uid="{6DE6D094-5B2C-4BEB-96BC-5C21BB0F9F6D}"/>
-    <hyperlink ref="J12" r:id="rId11" xr:uid="{E69D2F6C-04D4-4A87-9C99-E4623BE6A191}"/>
-    <hyperlink ref="J13" r:id="rId12" xr:uid="{68464EEE-80FE-4C5F-AEAE-112F37C094BB}"/>
-    <hyperlink ref="J14" r:id="rId13" xr:uid="{FE207A2A-0896-4539-A94E-4C76C5999E99}"/>
-    <hyperlink ref="J15" r:id="rId14" xr:uid="{10040561-D3C9-4F56-B280-64011AC446CB}"/>
-    <hyperlink ref="J16" r:id="rId15" xr:uid="{1E2F63B7-5CBC-49B7-99E5-19C6F5486E80}"/>
-    <hyperlink ref="J17" r:id="rId16" xr:uid="{715D4934-4D71-4FC1-BB6E-ADCF4950034C}"/>
-    <hyperlink ref="J18" r:id="rId17" xr:uid="{D4CCB1D0-09F2-4706-825D-99CE4CDBA11E}"/>
-    <hyperlink ref="J19" r:id="rId18" xr:uid="{F1F11CB3-6C24-406F-B644-B0D325CA6926}"/>
-    <hyperlink ref="J20" r:id="rId19" xr:uid="{C5283859-075D-4E14-AFFF-D80E37EA264A}"/>
-    <hyperlink ref="J21" r:id="rId20" xr:uid="{489FD3FC-3F37-4E36-A911-810F350C3720}"/>
-    <hyperlink ref="J22" r:id="rId21" xr:uid="{D40B3164-AF8B-4A52-957B-2EEF71337FDD}"/>
-    <hyperlink ref="J23" r:id="rId22" xr:uid="{2393D5E9-E57A-4D7B-8C85-2BFD236ACE16}"/>
-    <hyperlink ref="J24" r:id="rId23" xr:uid="{5843D405-52DE-4855-A557-EC44E2C37FA2}"/>
-    <hyperlink ref="J26" r:id="rId24" xr:uid="{30E82DF0-6CAD-44CB-89C7-01B4DE1D1FD3}"/>
-    <hyperlink ref="J27" r:id="rId25" xr:uid="{8EEA0F8F-CE8E-4DB7-9CFA-3C6DBE004F0A}"/>
-    <hyperlink ref="J28" r:id="rId26" xr:uid="{E50593B4-1219-4CA7-925E-A7070A83FF2F}"/>
-    <hyperlink ref="J29" r:id="rId27" xr:uid="{6480D2FD-75EF-44EE-99D0-DD57BEFCAB67}"/>
-    <hyperlink ref="J30" r:id="rId28" xr:uid="{CCE75B1B-8E52-43C3-8AED-315F55C95C97}"/>
-    <hyperlink ref="J31" r:id="rId29" xr:uid="{B7F9A4AB-3A4D-4712-BE2C-B2D88533FE3C}"/>
-    <hyperlink ref="J25" r:id="rId30" xr:uid="{06DFB3CB-B209-4712-A1CB-6CAD923C000C}"/>
-    <hyperlink ref="J32" r:id="rId31" xr:uid="{6B6778EE-AD28-494F-8872-20B2478B57D7}"/>
-    <hyperlink ref="J33" r:id="rId32" xr:uid="{889B760D-10E7-4158-87E7-03B22D3EF263}"/>
-    <hyperlink ref="J34" r:id="rId33" xr:uid="{1EF0392B-EAE0-4142-BDAB-4834B4AD6BB0}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{4B87C228-0DD4-4D05-AC70-AFD8CAF631E5}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{89FDCBF7-50D3-440F-BEDA-52BD32407FE4}"/>
+    <hyperlink ref="K4" r:id="rId3" xr:uid="{1A51576B-436E-41AA-B5C4-6471D93A4C8D}"/>
+    <hyperlink ref="K5" r:id="rId4" xr:uid="{1D0B1CE4-C7EE-4EE2-9BAD-26153E018D74}"/>
+    <hyperlink ref="K6" r:id="rId5" xr:uid="{B62D834C-4FC0-4CDD-B7F1-D7B9288F21B1}"/>
+    <hyperlink ref="K7" r:id="rId6" xr:uid="{FEFB7B95-C1F8-4155-808C-6E41EFB17F17}"/>
+    <hyperlink ref="K8" r:id="rId7" xr:uid="{1B97A028-EBD7-440C-BAAD-1DB7CE460F2C}"/>
+    <hyperlink ref="K9" r:id="rId8" xr:uid="{47B8D910-A5B5-4F0A-8B26-55329646996D}"/>
+    <hyperlink ref="K10" r:id="rId9" xr:uid="{281D3AA3-75C8-403A-8852-B7403F02E27F}"/>
+    <hyperlink ref="K11" r:id="rId10" xr:uid="{7EBCC98E-115E-49AE-9337-C07A0306B57D}"/>
+    <hyperlink ref="K12" r:id="rId11" xr:uid="{40332EE9-8D34-4B2A-9404-A1504B91D38C}"/>
+    <hyperlink ref="K13" r:id="rId12" xr:uid="{B291ECFE-99B4-4E60-A651-1440960D1F6C}"/>
+    <hyperlink ref="K14" r:id="rId13" xr:uid="{7D6A65CB-A4E5-4793-819D-CE89908E8052}"/>
+    <hyperlink ref="K15" r:id="rId14" xr:uid="{522F6141-644A-41C5-BB29-4E04261EC41F}"/>
+    <hyperlink ref="K16" r:id="rId15" xr:uid="{AF163991-2863-4A63-BA8F-EB5ABB54BC1E}"/>
+    <hyperlink ref="K17" r:id="rId16" xr:uid="{9FC9DAF6-06ED-4213-AE24-55AC595D70A1}"/>
+    <hyperlink ref="K18" r:id="rId17" xr:uid="{60AAF4ED-3B57-4EB0-A178-24E891E87E1C}"/>
+    <hyperlink ref="K19" r:id="rId18" xr:uid="{8F3E2F18-1628-4ACC-ACF8-C74B84549C41}"/>
+    <hyperlink ref="K20" r:id="rId19" xr:uid="{D3D39EF5-789D-4D2D-BD84-C3B4A690B8C8}"/>
+    <hyperlink ref="K21" r:id="rId20" xr:uid="{BE230D22-EFB8-43B0-98F5-F2BA40F0A7FA}"/>
+    <hyperlink ref="K22" r:id="rId21" xr:uid="{6E81F1C9-F637-40CC-BC3B-5FF128DB865C}"/>
+    <hyperlink ref="K23" r:id="rId22" xr:uid="{BFEC9A80-3EA0-41D9-BAF3-3349BD8EFDBA}"/>
+    <hyperlink ref="K24" r:id="rId23" xr:uid="{FCC51DB7-F1B3-40ED-AC5E-A4DD687ACE58}"/>
+    <hyperlink ref="K26" r:id="rId24" xr:uid="{B713D623-8512-4815-86B3-28C8CB778AB9}"/>
+    <hyperlink ref="K27" r:id="rId25" xr:uid="{028746EE-3D0B-464F-B359-E5F42476AB94}"/>
+    <hyperlink ref="K28" r:id="rId26" xr:uid="{1E14E936-42D6-482A-B80B-47703D94D2E1}"/>
+    <hyperlink ref="K29" r:id="rId27" xr:uid="{F6714CAF-CB19-42E3-8519-3A137E2D87FE}"/>
+    <hyperlink ref="K30" r:id="rId28" xr:uid="{D376FAB1-5D27-4149-915A-860190ED7215}"/>
+    <hyperlink ref="K31" r:id="rId29" xr:uid="{C1D9DC86-3F7A-4C30-A397-A9B120E6EC30}"/>
+    <hyperlink ref="K25" r:id="rId30" xr:uid="{B298054E-F073-4823-9616-52F74C8573DF}"/>
+    <hyperlink ref="K32" r:id="rId31" xr:uid="{171B7568-E8B6-4EA1-BB2C-0CA93A1180E6}"/>
+    <hyperlink ref="K33" r:id="rId32" xr:uid="{8DF66455-C096-4C43-9135-764475A45BD4}"/>
+    <hyperlink ref="K34" r:id="rId33" xr:uid="{283E5653-8BDB-44C9-A8B4-3A9D76B62DD4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>